<commit_message>
Adding custom models for planets and more.
</commit_message>
<xml_diff>
--- a/config/ctw.xlsx
+++ b/config/ctw.xlsx
@@ -8,20 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\github\copy-the-world\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE105055-6391-4E38-A138-C3F7F173A5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DBCC7C-7094-4340-BDE2-B355CE39719E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="3510" windowWidth="28800" windowHeight="15370" xr2:uid="{9A802DD3-F802-40DC-B7E9-C4F2EF300A0A}"/>
+    <workbookView xWindow="-38510" yWindow="10" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{9A802DD3-F802-40DC-B7E9-C4F2EF300A0A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Buildings" sheetId="1" r:id="rId1"/>
-    <sheet name="Levels" sheetId="2" r:id="rId2"/>
-    <sheet name="Rooms" sheetId="3" r:id="rId3"/>
-    <sheet name="Zones" sheetId="8" r:id="rId4"/>
-    <sheet name="PhoneBooths" sheetId="4" r:id="rId5"/>
-    <sheet name="Desks" sheetId="5" r:id="rId6"/>
-    <sheet name="Parking Lots" sheetId="10" r:id="rId7"/>
-    <sheet name="Parking spots" sheetId="6" r:id="rId8"/>
-    <sheet name="Car Chargers" sheetId="9" r:id="rId9"/>
+    <sheet name="Planets" sheetId="11" r:id="rId1"/>
+    <sheet name="Countries" sheetId="12" r:id="rId2"/>
+    <sheet name="Cities" sheetId="13" r:id="rId3"/>
+    <sheet name="Buildings" sheetId="1" r:id="rId4"/>
+    <sheet name="Levels" sheetId="2" r:id="rId5"/>
+    <sheet name="Rooms" sheetId="3" r:id="rId6"/>
+    <sheet name="Zones" sheetId="8" r:id="rId7"/>
+    <sheet name="PhoneBooths" sheetId="4" r:id="rId8"/>
+    <sheet name="Desks" sheetId="5" r:id="rId9"/>
+    <sheet name="Parking Lots" sheetId="10" r:id="rId10"/>
+    <sheet name="Parking spots" sheetId="6" r:id="rId11"/>
+    <sheet name="Car Chargers" sheetId="9" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="Buildings">Table1[]</definedName>
@@ -46,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="183">
   <si>
     <t>ID</t>
   </si>
@@ -526,6 +529,75 @@
   </si>
   <si>
     <t>D24</t>
+  </si>
+  <si>
+    <t>earth</t>
+  </si>
+  <si>
+    <t>mars</t>
+  </si>
+  <si>
+    <t>Earth</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Planet</t>
+  </si>
+  <si>
+    <t>netherlands</t>
+  </si>
+  <si>
+    <t>germany</t>
+  </si>
+  <si>
+    <t>belgium</t>
+  </si>
+  <si>
+    <t>usa</t>
+  </si>
+  <si>
+    <t>The Netherlands</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>United States Of America</t>
+  </si>
+  <si>
+    <t>hilversum</t>
+  </si>
+  <si>
+    <t>amsterdam</t>
+  </si>
+  <si>
+    <t>orlando</t>
+  </si>
+  <si>
+    <t>antwerp</t>
+  </si>
+  <si>
+    <t>Antwerp</t>
+  </si>
+  <si>
+    <t>Orlando</t>
+  </si>
+  <si>
+    <t>frankfurt</t>
+  </si>
+  <si>
+    <t>Frankfurt</t>
+  </si>
+  <si>
+    <t>CityTwin</t>
+  </si>
+  <si>
+    <t>Population</t>
   </si>
 </sst>
 </file>
@@ -722,11 +794,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}" name="Table1" displayName="Table1" ref="A1:G3" totalsRowShown="0">
-  <autoFilter ref="A1:G3" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8A1F753D-10BF-4B35-A59B-2603C486C4ED}" name="Table18" displayName="Table18" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{8A1F753D-10BF-4B35-A59B-2603C486C4ED}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5A58D701-BF8C-47A6-B49C-04EE5C5E3252}" name="ID"/>
+    <tableColumn id="7" xr3:uid="{D98B21AC-6125-4092-9512-08DBC3BF2CE0}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E23DC274-5C23-43CC-85ED-CD9D9C34F79D}" name="Table6" displayName="Table6" ref="A1:C13" totalsRowShown="0">
+  <autoFilter ref="A1:C13" xr:uid="{E23DC274-5C23-43CC-85ED-CD9D9C34F79D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B2F65E13-5342-4C93-9021-1B4E6C600843}" name="ID"/>
+    <tableColumn id="4" xr3:uid="{88F109CD-4DED-44D0-B3BF-2AC490306E44}" name="Building"/>
+    <tableColumn id="2" xr3:uid="{5CAD5D3B-3338-4D56-9059-03F7714D1A8C}" name="Parking"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FB4A760E-966B-4C6B-897C-D83902AF1BD8}" name="Table9" displayName="Table9" ref="A1:C7" totalsRowShown="0">
+  <autoFilter ref="A1:C7" xr:uid="{FB4A760E-966B-4C6B-897C-D83902AF1BD8}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{DE28C3ED-6D86-42AA-BB37-7B91C77F571F}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{138CA9E9-BCC2-4728-9A22-49F6B20512F6}" name="Building"/>
+    <tableColumn id="3" xr3:uid="{62C6B8C1-A833-458A-B7C4-ADD9C805A313}" name="Parking Spot"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{4E39A4B4-5299-4C0B-87C0-9534BB70D093}" name="Table1811" displayName="Table1811" ref="A1:C5" totalsRowShown="0">
+  <autoFilter ref="A1:C5" xr:uid="{4E39A4B4-5299-4C0B-87C0-9534BB70D093}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{CC2A72F3-D3FD-4E0B-9658-88A3C9132BA3}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{EA3C7334-0F95-4EED-B230-BB47635F502D}" name="Planet"/>
+    <tableColumn id="7" xr3:uid="{A9AC266E-232B-47AD-8D74-EC32ED101E1D}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{A47D8A87-7E9C-4E91-8A1A-F1FDCE8AA55D}" name="Table181112" displayName="Table181112" ref="A1:D6" totalsRowShown="0">
+  <autoFilter ref="A1:D6" xr:uid="{A47D8A87-7E9C-4E91-8A1A-F1FDCE8AA55D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{8332FE7F-DA71-4798-A0D2-8F23EC409017}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{B8D8DBDD-3DAF-4CC9-B4C0-505D964BA019}" name="Country"/>
+    <tableColumn id="7" xr3:uid="{322021A7-CD17-43A9-86EB-91EBCFBE8F27}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{D2525123-156E-466F-A8FC-37F43AFC4D19}" name="Population"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}" name="Table1" displayName="Table1" ref="A1:H3" totalsRowShown="0">
+  <autoFilter ref="A1:H3" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{CC0D9068-E39E-4DCA-BDFD-DAB0927E9F90}" name="ID"/>
     <tableColumn id="7" xr3:uid="{473F1CEC-5290-4EA9-9033-5EEB95FA3E3B}" name="Name"/>
+    <tableColumn id="9" xr3:uid="{D64CD8FC-A734-4663-92B6-9BBF02A5290A}" name="CityTwin"/>
     <tableColumn id="2" xr3:uid="{D95F549B-1C42-4BE4-9990-8B309CBB714B}" name="Country"/>
     <tableColumn id="3" xr3:uid="{3D62CC33-189C-4765-A3A2-C5691204023F}" name="City"/>
     <tableColumn id="4" xr3:uid="{ECF2DC82-76C7-424B-A6F4-43CD8C67FFFA}" name="PostalCode"/>
@@ -737,7 +870,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0">
   <autoFilter ref="A1:B5" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}"/>
   <tableColumns count="2">
@@ -748,7 +881,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}" name="Table3" displayName="Table3" ref="A1:E68" totalsRowShown="0">
   <autoFilter ref="A1:E68" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E26">
@@ -765,7 +898,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}" name="Table8" displayName="Table8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="A1:D8" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}"/>
   <tableColumns count="4">
@@ -778,7 +911,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CFA3B6A6-B2B7-4A7E-AD44-23D09DDF8633}" name="Table4" displayName="Table4" ref="A1:E4" totalsRowShown="0">
   <autoFilter ref="A1:E4" xr:uid="{CFA3B6A6-B2B7-4A7E-AD44-23D09DDF8633}"/>
   <tableColumns count="5">
@@ -792,7 +925,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}" name="Table5" displayName="Table5" ref="A1:D25" totalsRowShown="0">
   <autoFilter ref="A1:D25" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}"/>
   <tableColumns count="4">
@@ -802,30 +935,6 @@
     <tableColumn id="3" xr3:uid="{5467CA94-5087-4D6C-9991-8475D8A1C3B6}" name="Level"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E23DC274-5C23-43CC-85ED-CD9D9C34F79D}" name="Table6" displayName="Table6" ref="A1:C13" totalsRowShown="0">
-  <autoFilter ref="A1:C13" xr:uid="{E23DC274-5C23-43CC-85ED-CD9D9C34F79D}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B2F65E13-5342-4C93-9021-1B4E6C600843}" name="ID"/>
-    <tableColumn id="4" xr3:uid="{88F109CD-4DED-44D0-B3BF-2AC490306E44}" name="Building"/>
-    <tableColumn id="2" xr3:uid="{5CAD5D3B-3338-4D56-9059-03F7714D1A8C}" name="Parking"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{FB4A760E-966B-4C6B-897C-D83902AF1BD8}" name="Table9" displayName="Table9" ref="A1:C7" totalsRowShown="0">
-  <autoFilter ref="A1:C7" xr:uid="{FB4A760E-966B-4C6B-897C-D83902AF1BD8}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{DE28C3ED-6D86-42AA-BB37-7B91C77F571F}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{138CA9E9-BCC2-4728-9A22-49F6B20512F6}" name="Building"/>
-    <tableColumn id="3" xr3:uid="{62C6B8C1-A833-458A-B7C4-ADD9C805A313}" name="Parking Spot"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1125,23 +1234,622 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA510EF-B804-42E2-B8DD-C1D72D4A589B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C859A245-3C90-4B7C-9DD7-F25A178C6105}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F0EEF64-2025-4004-A843-169C6D1A285E}">
+          <x14:formula1>
+            <xm:f>Buildings!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D3A0EF-4BE8-40EA-8F85-0C9098AE9314}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="9.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{40C1D587-0DE4-4C48-974E-181AAABF8FAF}">
+          <x14:formula1>
+            <xm:f>'Parking Lots'!$A$2</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C13</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{432E18F6-F329-49DE-B154-489A9CD545F1}">
+          <x14:formula1>
+            <xm:f>Buildings!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D64CDF-AE10-41CD-A603-F1146F496055}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F1A8623-C40F-4361-BEBF-434E53520A32}">
+          <x14:formula1>
+            <xm:f>Buildings!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B7</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ADD32B8-2F64-46F1-9F33-48DE9BD82168}">
+          <x14:formula1>
+            <xm:f>'Parking spots'!$A$2:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C7</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABCCC7B-39F1-4D4A-A87E-82A807CA683D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4682490A-1B57-4660-8EE0-EDE01CD36C88}">
+          <x14:formula1>
+            <xm:f>Planets!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73738864-F428-4908-AB05-D87D631C82A3}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>90261</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>821752</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4">
+        <v>284817</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5">
+        <v>506922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6">
+        <v>753056</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BAEB20D-CE9B-46B6-B663-07B4F73E88EC}">
+          <x14:formula1>
+            <xm:f>Countries!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F496CE3C-4FCB-42A2-AD40-19A0C25E579C}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" customWidth="1"/>
+    <col min="4" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="19.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1149,22 +1857,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1172,22 +1883,25 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1195,18 +1909,21 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1216,10 +1933,22 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{795A2530-FDFF-45C7-BE87-94418D306CC7}">
+          <x14:formula1>
+            <xm:f>Cities!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C91AB9F-3898-47A2-861B-71AFD5DEB950}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1292,7 +2021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1535539-AB89-4B69-BFDB-9E52D2F3597C}">
   <dimension ref="A1:E68"/>
   <sheetViews>
@@ -2338,7 +3067,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBD7FD1-964D-45AB-A9E2-51A514C7A6F2}">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -2484,7 +3213,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24169BE6-9848-46E7-9522-D69D04E2D41F}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -2585,7 +3314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CFE91E-FDA2-45F8-B52A-C8C5712828C8}">
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -2973,351 +3702,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C859A245-3C90-4B7C-9DD7-F25A178C6105}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.90625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2F0EEF64-2025-4004-A843-169C6D1A285E}">
-          <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D3A0EF-4BE8-40EA-8F85-0C9098AE9314}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="9.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>148</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>149</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>150</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>152</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>153</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>154</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{40C1D587-0DE4-4C48-974E-181AAABF8FAF}">
-          <x14:formula1>
-            <xm:f>'Parking Lots'!$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C13</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{432E18F6-F329-49DE-B154-489A9CD545F1}">
-          <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B13</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02D64CDF-AE10-41CD-A603-F1146F496055}">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F1A8623-C40F-4361-BEBF-434E53520A32}">
-          <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7ADD32B8-2F64-46F1-9F33-48DE9BD82168}">
-          <x14:formula1>
-            <xm:f>'Parking spots'!$A$2:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C7</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding desks/rooms for locations
</commit_message>
<xml_diff>
--- a/config/ctw.xlsx
+++ b/config/ctw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\github\copy-the-world\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DBCC7C-7094-4340-BDE2-B355CE39719E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC64F12D-C7A8-4158-9788-3509F5C97EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="10" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{9A802DD3-F802-40DC-B7E9-C4F2EF300A0A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="8" xr2:uid="{9A802DD3-F802-40DC-B7E9-C4F2EF300A0A}"/>
   </bookViews>
   <sheets>
     <sheet name="Planets" sheetId="11" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Cities" sheetId="13" r:id="rId3"/>
     <sheet name="Buildings" sheetId="1" r:id="rId4"/>
     <sheet name="Levels" sheetId="2" r:id="rId5"/>
-    <sheet name="Rooms" sheetId="3" r:id="rId6"/>
-    <sheet name="Zones" sheetId="8" r:id="rId7"/>
+    <sheet name="Zones" sheetId="8" r:id="rId6"/>
+    <sheet name="Rooms" sheetId="3" r:id="rId7"/>
     <sheet name="PhoneBooths" sheetId="4" r:id="rId8"/>
     <sheet name="Desks" sheetId="5" r:id="rId9"/>
     <sheet name="Parking Lots" sheetId="10" r:id="rId10"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="212">
   <si>
     <t>ID</t>
   </si>
@@ -598,6 +598,93 @@
   </si>
   <si>
     <t>Population</t>
+  </si>
+  <si>
+    <t>ORL</t>
+  </si>
+  <si>
+    <t>Xpirit Orlando</t>
+  </si>
+  <si>
+    <t>FRK</t>
+  </si>
+  <si>
+    <t>Xpirit Germany</t>
+  </si>
+  <si>
+    <t>28.4616643,-81.367894</t>
+  </si>
+  <si>
+    <t>50.1121608,8.656647</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>Xpirit Belgium</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>51.2092121,4.4439108</t>
+  </si>
+  <si>
+    <t>OptimusPrime</t>
+  </si>
+  <si>
+    <t>Bumblebee</t>
+  </si>
+  <si>
+    <t>Cliffjumper</t>
+  </si>
+  <si>
+    <t>Wheeljack</t>
+  </si>
+  <si>
+    <t>Prowl</t>
+  </si>
+  <si>
+    <t>Bilbo</t>
+  </si>
+  <si>
+    <t>Frodo</t>
+  </si>
+  <si>
+    <t>Samwise</t>
+  </si>
+  <si>
+    <t>Meriadoc</t>
+  </si>
+  <si>
+    <t>Belladonna</t>
+  </si>
+  <si>
+    <t>Peregrin</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>SpiderMan</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>Hulk</t>
+  </si>
+  <si>
+    <t>Daredevil</t>
+  </si>
+  <si>
+    <t>Punisher</t>
   </si>
 </sst>
 </file>
@@ -702,7 +789,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -713,6 +800,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -854,8 +942,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}" name="Table1" displayName="Table1" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}" name="Table1" displayName="Table1" ref="A1:H6" totalsRowShown="0">
+  <autoFilter ref="A1:H6" xr:uid="{286E368C-FE77-4E6B-9074-2516FF806E1F}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{CC0D9068-E39E-4DCA-BDFD-DAB0927E9F90}" name="ID"/>
     <tableColumn id="7" xr3:uid="{473F1CEC-5290-4EA9-9033-5EEB95FA3E3B}" name="Name"/>
@@ -871,8 +959,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}" name="Table2" displayName="Table2" ref="A1:B5" totalsRowShown="0">
-  <autoFilter ref="A1:B5" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}" name="Table2" displayName="Table2" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{16DBF3CF-DFAA-4226-A74F-3FF95F5614F0}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{FE7D0D47-DC0C-43F7-81AE-4C733CE27A01}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{BCB2ED7B-FC9C-482A-B7E5-40AD2BC48DEC}" name="Building"/>
@@ -882,8 +970,21 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}" name="Table3" displayName="Table3" ref="A1:E68" totalsRowShown="0">
-  <autoFilter ref="A1:E68" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}" name="Table8" displayName="Table8" ref="A1:D10" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="A1:D10" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{E85DA0FE-32F9-4428-811C-D5E3ED923FA6}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{B68FA473-2AD7-4BFA-84E4-9A8F85F569D8}" name="Building" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{C574EEC4-AF96-4547-8821-86BDB9619A97}" name="Name"/>
+    <tableColumn id="4" xr3:uid="{76325719-C930-4888-A2C5-86FF12E71230}" name="Level"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}" name="Table3" displayName="Table3" ref="A1:E85" totalsRowShown="0">
+  <autoFilter ref="A1:E85" xr:uid="{88B3C328-C0A5-41A4-BF4D-2C029E2BF87E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E26">
     <sortCondition ref="A1:A26"/>
   </sortState>
@@ -893,19 +994,6 @@
     <tableColumn id="3" xr3:uid="{553B7577-C52D-4256-9C71-F31A3AAD5A91}" name="Name"/>
     <tableColumn id="5" xr3:uid="{94606806-F489-4FB4-BB42-58D2B96D413F}" name="Zone"/>
     <tableColumn id="4" xr3:uid="{C0AB62C2-5551-4DDB-A88E-E06B3F126747}" name="Level"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}" name="Table8" displayName="Table8" ref="A1:D8" totalsRowShown="0" headerRowDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="A1:D8" xr:uid="{7ACCEDDF-2DE4-49BC-B6EC-2DAB6698B40C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E85DA0FE-32F9-4428-811C-D5E3ED923FA6}" name="ID"/>
-    <tableColumn id="2" xr3:uid="{B68FA473-2AD7-4BFA-84E4-9A8F85F569D8}" name="Building" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{C574EEC4-AF96-4547-8821-86BDB9619A97}" name="Name"/>
-    <tableColumn id="4" xr3:uid="{76325719-C930-4888-A2C5-86FF12E71230}" name="Level"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -926,8 +1014,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}" name="Table5" displayName="Table5" ref="A1:D25" totalsRowShown="0">
-  <autoFilter ref="A1:D25" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}" name="Table5" displayName="Table5" ref="A1:D95" totalsRowShown="0">
+  <autoFilter ref="A1:D95" xr:uid="{AB610C45-6A0D-43F1-BB8E-3C9A91BF956F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4054AA3F-5E8D-47BD-BF01-D7AEE18D98CB}" name="ID"/>
     <tableColumn id="2" xr3:uid="{350C66A8-75EE-4471-896F-5EEE3965EC40}" name="Building"/>
@@ -1833,10 +1921,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F496CE3C-4FCB-42A2-AD40-19A0C25E579C}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1927,6 +2015,66 @@
         <v>21</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B4" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" t="s">
+        <v>190</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H6" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1940,7 +2088,7 @@
           <x14:formula1>
             <xm:f>Cities!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C3</xm:sqref>
+          <xm:sqref>C2:C6</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1950,10 +2098,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C91AB9F-3898-47A2-861B-71AFD5DEB950}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1999,6 +2147,54 @@
       </c>
       <c r="B5" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="4">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="4">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="4">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2011,9 +2207,9 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{29A5EA50-D43C-4FF8-A20F-5E0D33A100FB}">
           <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
+            <xm:f>Buildings!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B5</xm:sqref>
+          <xm:sqref>B2:B11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2022,15 +2218,190 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1535539-AB89-4B69-BFDB-9E52D2F3597C}">
-  <dimension ref="A1:E68"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBD7FD1-964D-45AB-A9E2-51A514C7A6F2}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="9.453125" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE597BE1-6971-4332-9870-A7224090FC9A}">
+          <x14:formula1>
+            <xm:f>Buildings!$A$2:$A$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B10</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1535539-AB89-4B69-BFDB-9E52D2F3597C}">
+  <dimension ref="A1:E85"/>
+  <sheetViews>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.453125" customWidth="1"/>
     <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.1796875" customWidth="1"/>
@@ -3038,6 +3409,262 @@
       </c>
       <c r="E68">
         <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>193</v>
+      </c>
+      <c r="B69" t="s">
+        <v>183</v>
+      </c>
+      <c r="C69" t="s">
+        <v>193</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>194</v>
+      </c>
+      <c r="B70" t="s">
+        <v>183</v>
+      </c>
+      <c r="C70" t="s">
+        <v>194</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>195</v>
+      </c>
+      <c r="B71" t="s">
+        <v>183</v>
+      </c>
+      <c r="C71" t="s">
+        <v>195</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>196</v>
+      </c>
+      <c r="B72" t="s">
+        <v>183</v>
+      </c>
+      <c r="C72" t="s">
+        <v>196</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>197</v>
+      </c>
+      <c r="B73" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" t="s">
+        <v>197</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>198</v>
+      </c>
+      <c r="B74" t="s">
+        <v>185</v>
+      </c>
+      <c r="C74" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" t="s">
+        <v>204</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>199</v>
+      </c>
+      <c r="B75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
+        <v>199</v>
+      </c>
+      <c r="D75" t="s">
+        <v>204</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>200</v>
+      </c>
+      <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" t="s">
+        <v>200</v>
+      </c>
+      <c r="D76" t="s">
+        <v>204</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>201</v>
+      </c>
+      <c r="B77" t="s">
+        <v>185</v>
+      </c>
+      <c r="C77" t="s">
+        <v>201</v>
+      </c>
+      <c r="D77" t="s">
+        <v>205</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>202</v>
+      </c>
+      <c r="B78" t="s">
+        <v>185</v>
+      </c>
+      <c r="C78" t="s">
+        <v>202</v>
+      </c>
+      <c r="D78" t="s">
+        <v>205</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>203</v>
+      </c>
+      <c r="B79" t="s">
+        <v>185</v>
+      </c>
+      <c r="C79" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" t="s">
+        <v>205</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>206</v>
+      </c>
+      <c r="B80" t="s">
+        <v>189</v>
+      </c>
+      <c r="C80" t="s">
+        <v>206</v>
+      </c>
+      <c r="E80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" t="s">
+        <v>189</v>
+      </c>
+      <c r="C81" t="s">
+        <v>207</v>
+      </c>
+      <c r="E81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>208</v>
+      </c>
+      <c r="B82" t="s">
+        <v>189</v>
+      </c>
+      <c r="C82" t="s">
+        <v>208</v>
+      </c>
+      <c r="E82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>209</v>
+      </c>
+      <c r="B83" t="s">
+        <v>189</v>
+      </c>
+      <c r="C83" t="s">
+        <v>209</v>
+      </c>
+      <c r="E83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>210</v>
+      </c>
+      <c r="B84" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" t="s">
+        <v>210</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>211</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+      <c r="C85" t="s">
+        <v>211</v>
+      </c>
+      <c r="E85">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3051,161 +3678,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{493E7F9D-254A-45D1-AD23-64FD31EC9A50}">
           <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
+            <xm:f>Buildings!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B68</xm:sqref>
+          <xm:sqref>B2:B85</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{91AAD73E-737E-49C3-B84B-7501CFDA2DEB}">
           <x14:formula1>
-            <xm:f>Zones!$A$2:$A$8</xm:f>
+            <xm:f>Zones!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D68</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBD7FD1-964D-45AB-A9E2-51A514C7A6F2}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="9.453125" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>129</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>131</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>132</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>133</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EE597BE1-6971-4332-9870-A7224090FC9A}">
-          <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
+          <xm:sqref>D2:D85</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3316,10 +3797,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CFE91E-FDA2-45F8-B52A-C8C5712828C8}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3675,6 +4156,836 @@
       </c>
       <c r="D25">
         <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>183</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>183</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>183</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>183</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>183</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>183</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>183</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>183</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>183</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>29</v>
+      </c>
+      <c r="B42" t="s">
+        <v>183</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>30</v>
+      </c>
+      <c r="B43" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>31</v>
+      </c>
+      <c r="B44" t="s">
+        <v>183</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" t="s">
+        <v>183</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" t="s">
+        <v>183</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>37</v>
+      </c>
+      <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>183</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>26</v>
+      </c>
+      <c r="B52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" t="s">
+        <v>204</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>185</v>
+      </c>
+      <c r="C53" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>28</v>
+      </c>
+      <c r="B54" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" t="s">
+        <v>204</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" t="s">
+        <v>204</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" t="s">
+        <v>185</v>
+      </c>
+      <c r="C57" t="s">
+        <v>204</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>32</v>
+      </c>
+      <c r="B58" t="s">
+        <v>185</v>
+      </c>
+      <c r="C58" t="s">
+        <v>204</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>34</v>
+      </c>
+      <c r="B60" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" t="s">
+        <v>204</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" t="s">
+        <v>185</v>
+      </c>
+      <c r="C61" t="s">
+        <v>204</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>26</v>
+      </c>
+      <c r="B62" t="s">
+        <v>185</v>
+      </c>
+      <c r="C62" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" t="s">
+        <v>205</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C65" t="s">
+        <v>205</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>30</v>
+      </c>
+      <c r="B66" t="s">
+        <v>185</v>
+      </c>
+      <c r="C66" t="s">
+        <v>205</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" t="s">
+        <v>185</v>
+      </c>
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68" t="s">
+        <v>185</v>
+      </c>
+      <c r="C68" t="s">
+        <v>205</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69" t="s">
+        <v>185</v>
+      </c>
+      <c r="C69" t="s">
+        <v>205</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>34</v>
+      </c>
+      <c r="B70" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" t="s">
+        <v>205</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
+        <v>205</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" t="s">
+        <v>189</v>
+      </c>
+      <c r="D72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>189</v>
+      </c>
+      <c r="D73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>28</v>
+      </c>
+      <c r="B74" t="s">
+        <v>189</v>
+      </c>
+      <c r="D74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>29</v>
+      </c>
+      <c r="B75" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>30</v>
+      </c>
+      <c r="B76" t="s">
+        <v>189</v>
+      </c>
+      <c r="D76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" t="s">
+        <v>189</v>
+      </c>
+      <c r="D77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" t="s">
+        <v>189</v>
+      </c>
+      <c r="D78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>33</v>
+      </c>
+      <c r="B79" t="s">
+        <v>189</v>
+      </c>
+      <c r="D79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>26</v>
+      </c>
+      <c r="B80" t="s">
+        <v>189</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81" t="s">
+        <v>189</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>28</v>
+      </c>
+      <c r="B82" t="s">
+        <v>189</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>29</v>
+      </c>
+      <c r="B83" t="s">
+        <v>189</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>30</v>
+      </c>
+      <c r="B84" t="s">
+        <v>189</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" t="s">
+        <v>189</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" t="s">
+        <v>189</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>189</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>26</v>
+      </c>
+      <c r="B88" t="s">
+        <v>189</v>
+      </c>
+      <c r="D88">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>27</v>
+      </c>
+      <c r="B89" t="s">
+        <v>189</v>
+      </c>
+      <c r="D89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>28</v>
+      </c>
+      <c r="B90" t="s">
+        <v>189</v>
+      </c>
+      <c r="D90">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>29</v>
+      </c>
+      <c r="B91" t="s">
+        <v>189</v>
+      </c>
+      <c r="D91">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>30</v>
+      </c>
+      <c r="B92" t="s">
+        <v>189</v>
+      </c>
+      <c r="D92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93" t="s">
+        <v>189</v>
+      </c>
+      <c r="D93">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" t="s">
+        <v>189</v>
+      </c>
+      <c r="D94">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>33</v>
+      </c>
+      <c r="B95" t="s">
+        <v>189</v>
+      </c>
+      <c r="D95">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -3688,15 +4999,15 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0F6C4BAD-05B0-4AAA-BD07-A1A2565B6D1F}">
           <x14:formula1>
-            <xm:f>Buildings!$A$2:$A$3</xm:f>
+            <xm:f>Buildings!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B25</xm:sqref>
+          <xm:sqref>B2:B95</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECF9E65C-C06A-4F19-968E-E461C4F0B928}">
           <x14:formula1>
-            <xm:f>Zones!$A$2:$A$8</xm:f>
+            <xm:f>Zones!$A$2:$A$10</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C25</xm:sqref>
+          <xm:sqref>C2:C95</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>